<commit_message>
Correct errors in spreadsheet fixture
</commit_message>
<xml_diff>
--- a/tests/fixtures/simplicity.xlsx
+++ b/tests/fixtures/simplicity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wusher/repository/otoole/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95C3A53-B49E-0B47-B5F0-7377D1E44C9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C461D9-87EA-9944-B0D7-32BCD10D303A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="-7340" windowWidth="51200" windowHeight="28340" tabRatio="966" firstSheet="30" activeTab="59" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33600" yWindow="-7340" windowWidth="51200" windowHeight="28340" tabRatio="966" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STORAGE" sheetId="6" r:id="rId1"/>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="68">
   <si>
     <t>EMISSION</t>
   </si>
@@ -3907,74 +3907,14 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:BE1"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="AA23" sqref="AA23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1"/>
-      <c r="AD1" s="1"/>
-      <c r="AE1" s="1"/>
-      <c r="AF1" s="1"/>
-      <c r="AG1" s="1"/>
-      <c r="AH1" s="1"/>
-      <c r="AI1" s="1"/>
-      <c r="AJ1" s="1"/>
-      <c r="AK1" s="1"/>
-      <c r="AL1" s="1"/>
-      <c r="AM1" s="1"/>
-      <c r="AN1" s="1"/>
-      <c r="AO1" s="1"/>
-      <c r="AP1" s="1"/>
-      <c r="AQ1" s="1"/>
-      <c r="AR1" s="1"/>
-      <c r="AS1" s="1"/>
-      <c r="AT1" s="1"/>
-      <c r="AU1" s="1"/>
-      <c r="AV1" s="1"/>
-      <c r="AW1" s="1"/>
-      <c r="AX1" s="1"/>
-      <c r="AY1" s="1"/>
-      <c r="AZ1" s="1"/>
-      <c r="BA1" s="1"/>
-      <c r="BB1" s="1"/>
-      <c r="BC1" s="1"/>
-      <c r="BD1" s="1"/>
-      <c r="BE1" s="1"/>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -3984,7 +3924,7 @@
   <dimension ref="A1:B4034"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B18"/>
+      <selection activeCell="AB62" sqref="AB62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5805,21 +5745,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A6:A7"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -6010,7 +5950,7 @@
   <dimension ref="A1:AD5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:AD1"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7389,7 +7329,7 @@
   <dimension ref="A1:AD37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="V63" sqref="V63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11173,14 +11113,14 @@
   <dimension ref="A1:AD82"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="P36" sqref="P36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="28" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="5.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -11192,85 +11132,88 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1">
         <v>2014</v>
       </c>
-      <c r="D1">
+      <c r="E1">
         <v>2015</v>
       </c>
-      <c r="E1">
+      <c r="F1">
         <v>2016</v>
       </c>
-      <c r="F1">
+      <c r="G1">
         <v>2017</v>
       </c>
-      <c r="G1">
+      <c r="H1">
         <v>2018</v>
       </c>
-      <c r="H1">
+      <c r="I1">
         <v>2019</v>
       </c>
-      <c r="I1">
+      <c r="J1">
         <v>2020</v>
       </c>
-      <c r="J1">
+      <c r="K1">
         <v>2021</v>
       </c>
-      <c r="K1">
+      <c r="L1">
         <v>2022</v>
       </c>
-      <c r="L1">
+      <c r="M1">
         <v>2023</v>
       </c>
-      <c r="M1">
+      <c r="N1">
         <v>2024</v>
       </c>
-      <c r="N1">
+      <c r="O1">
         <v>2025</v>
       </c>
-      <c r="O1">
+      <c r="P1">
         <v>2026</v>
       </c>
-      <c r="P1">
+      <c r="Q1">
         <v>2027</v>
       </c>
-      <c r="Q1">
+      <c r="R1">
         <v>2028</v>
       </c>
-      <c r="R1">
+      <c r="S1">
         <v>2029</v>
       </c>
-      <c r="S1">
+      <c r="T1">
         <v>2030</v>
       </c>
-      <c r="T1">
+      <c r="U1">
         <v>2031</v>
       </c>
-      <c r="U1">
+      <c r="V1">
         <v>2032</v>
       </c>
-      <c r="V1">
+      <c r="W1">
         <v>2033</v>
       </c>
-      <c r="W1">
+      <c r="X1">
         <v>2034</v>
       </c>
-      <c r="X1">
+      <c r="Y1">
         <v>2035</v>
       </c>
-      <c r="Y1">
+      <c r="Z1">
         <v>2036</v>
       </c>
-      <c r="Z1">
+      <c r="AA1">
         <v>2037</v>
       </c>
-      <c r="AA1">
+      <c r="AB1">
         <v>2038</v>
       </c>
-      <c r="AB1">
+      <c r="AC1">
         <v>2039</v>
       </c>
-      <c r="AC1">
+      <c r="AD1">
         <v>2040</v>
       </c>
     </row>
@@ -13773,7 +13716,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="A1:XFD1048576"/>
+      <selection activeCell="K64" sqref="K64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16412,7 +16355,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:A1422"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -21271,8 +21214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2E00-000000000000}">
   <dimension ref="A1:AB7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AC37" sqref="AC37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>